<commit_message>
[PV-272][WIP] Get tests running after several changes without running them
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968A35A2-732A-E14B-B9C9-922465D37B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48488CCA-E69B-2244-A900-D9E31D212BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV-Test-01" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>Level #</t>
   </si>
   <si>
-    <t>Task Name</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -550,8 +550,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -574,45 +574,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="4">
         <v>44927</v>
@@ -628,16 +628,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E3" s="4">
         <v>44928</v>
@@ -653,16 +653,16 @@
     </row>
     <row r="4" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="4">
         <v>44928</v>
@@ -678,16 +678,16 @@
     </row>
     <row r="5" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E5" s="4">
         <v>44928</v>
@@ -696,7 +696,7 @@
         <v>44939</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
@@ -705,16 +705,16 @@
     </row>
     <row r="6" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E6" s="4">
         <v>44942</v>
@@ -723,7 +723,7 @@
         <v>44946</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
@@ -732,16 +732,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4">
         <v>44949</v>
@@ -750,7 +750,7 @@
         <v>44953</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5"/>
@@ -759,16 +759,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4">
         <v>44956</v>
@@ -777,7 +777,7 @@
         <v>44967</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>
@@ -794,7 +794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DABCD83-856B-ED46-BCE9-48AECEB468B0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
[PV-94][WIP] Support for plans without sticky-ids or levels
Changes...
- Removed check for completeness (and associated test) of a mapping type in plan_reader.py as this is going to be hard-coded and so isn't going to depend upon the DB being updated correctly.
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48488CCA-E69B-2244-A900-D9E31D212BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90FBDA3-C894-BA4E-9ADA-E95952728F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,21 +23,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
-    <t>Unique Sticky ID</t>
-  </si>
-  <si>
     <t>Level #</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Finish</t>
-  </si>
-  <si>
     <t>Predecessors</t>
   </si>
   <si>
@@ -119,7 +110,16 @@
     <t>6</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Row ID</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -249,9 +249,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +289,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -395,7 +395,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -537,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,7 +551,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -568,51 +568,51 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4">
         <v>44927</v>
@@ -628,16 +628,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4">
         <v>44928</v>
@@ -653,16 +653,16 @@
     </row>
     <row r="4" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4">
         <v>44928</v>
@@ -678,16 +678,16 @@
     </row>
     <row r="5" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4">
         <v>44928</v>
@@ -696,7 +696,7 @@
         <v>44939</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
@@ -705,16 +705,16 @@
     </row>
     <row r="6" spans="1:11" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4">
         <v>44942</v>
@@ -723,7 +723,7 @@
         <v>44946</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="5"/>
@@ -732,16 +732,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="4">
         <v>44949</v>
@@ -750,7 +750,7 @@
         <v>44953</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="5"/>
@@ -759,16 +759,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4">
         <v>44956</v>
@@ -777,7 +777,7 @@
         <v>44967</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="5"/>

</xml_diff>

<commit_message>
[PV-350][WIP] Replace hard coding of visual height with calculated value
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files/PV-Test-01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser_2023_02/plan_visual_django/tests/resources/input_files/excel_plan_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90FBDA3-C894-BA4E-9ADA-E95952728F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B43E73-A3DC-B54D-A5F2-98B4788CC979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="500" windowWidth="29400" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,16 +110,16 @@
     <t>6</t>
   </si>
   <si>
-    <t>Row ID</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Finish</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>

</xml_diff>